<commit_message>
Lavet test  om vi kan undgåå at køre ting to gange
</commit_message>
<xml_diff>
--- a/AAMK Hamid.xlsx
+++ b/AAMK Hamid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon ik mig\Desktop\9. Semester\Arbejdsmarkeds projekt\Empirisk-SFC-model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjkss\Desktop\9. semester\Empirisk-SFC-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13080B8A-DC3E-46DE-9467-399E0453D8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593F99A2-D8E9-44BC-825B-CB12DCF0C428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="517">
   <si>
     <t>IBA_h</t>
   </si>
@@ -1576,9 +1576,6 @@
     <t>wage_ds</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>inflation</t>
   </si>
   <si>
@@ -1974,9 +1971,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:QO68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="141" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="QE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="QP55" sqref="QP55"/>
+      <selection pane="topRight" activeCell="QN12" sqref="QN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3345,13 +3342,13 @@
         <v>513</v>
       </c>
       <c r="QM1" t="s">
+        <v>514</v>
+      </c>
+      <c r="QN1" t="s">
         <v>515</v>
       </c>
-      <c r="QN1" t="s">
+      <c r="QO1" t="s">
         <v>516</v>
-      </c>
-      <c r="QO1" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:457" ht="15.75" x14ac:dyDescent="0.25">
@@ -4717,8 +4714,8 @@
       <c r="QL2" s="5">
         <v>73.604820000000004</v>
       </c>
-      <c r="QM2" t="s">
-        <v>514</v>
+      <c r="QM2">
+        <v>0</v>
       </c>
       <c r="QN2" s="5">
         <v>73.604820000000004</v>
@@ -6090,8 +6087,8 @@
       <c r="QL3" s="5">
         <v>75.203680000000006</v>
       </c>
-      <c r="QM3" t="s">
-        <v>514</v>
+      <c r="QM3">
+        <v>0</v>
       </c>
       <c r="QN3" s="5">
         <v>75.203680000000006</v>
@@ -7463,8 +7460,8 @@
       <c r="QL4" s="5">
         <v>73.585819999999998</v>
       </c>
-      <c r="QM4" t="s">
-        <v>514</v>
+      <c r="QM4">
+        <v>0</v>
       </c>
       <c r="QN4" s="5">
         <v>73.585819999999998</v>
@@ -8836,8 +8833,8 @@
       <c r="QL5" s="5">
         <v>73.624889999999994</v>
       </c>
-      <c r="QM5" t="s">
-        <v>514</v>
+      <c r="QM5">
+        <v>0</v>
       </c>
       <c r="QN5" s="5">
         <v>73.624889999999994</v>

</xml_diff>